<commit_message>
Thêm bổ sung 2 trường mới vào màn hình AS0053
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/AS0053_Cap nhat nhan vien.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/AS0053_Cap nhat nhan vien.xlsx
@@ -1087,7 +1087,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="252">
   <si>
     <t>Detail Design</t>
   </si>
@@ -1890,19 +1890,55 @@
     <t>Disabled khi ở màn hình Edit và View</t>
   </si>
   <si>
+    <t>Thêm mới trường SipPassword vào AT1103 áp dụng cho CustomizeIndex 51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm mới trường SipID vào AT1103 áp dụng cho CustomizeIndex 51 </t>
+  </si>
+  <si>
+    <t>Textbox này được thêm mới trong màn hình cũ. Disabled khi ở màn hình Edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmployeeID, FullName, DepartmentID, EmployeeTypeID, HireDate, EndDate, BirthDay, Address, Tel, Fax, Email, IsUserID, SipID, SipPassword </t>
+  </si>
+  <si>
+    <t>@SQL0003</t>
+  </si>
+  <si>
+    <t>INSERT INTO AT1103(DivisionID, EmployeeID, FullName,
+      DepartmentID, EmployeeTypeID, HireDate,EndDate,
+      BirthDay,Address, Tel, Fax, Email,IsUserID,Disabled,
+CreateDate,CreateUserID,LastModifyUserID, LastModifyDate,
+      IsCommon) 
+VALUES (@DivisionID, @EmployeeID, @FullName, @DepartmentID, @EmployeeTypeID, @HireDate, @EndDate, @BirthDay, @Address, @Tel, @Fax, @Email, @IsUserID, @SipID, @SipPassword)</t>
+  </si>
+  <si>
+    <t>@DivisionID
+@EmployeeID @FullName @DepartmentID @EmployeeTypeID @HireDate @EndDate @BirthDay
+@Address
+@Tel 
+@Fax 
+@Email
+@IsUserID
+@SipID
+@SipPassword</t>
+  </si>
+  <si>
+    <t>@@DivisionID @@EmployeeID @@FullName @@DepartmentID @@EmployeeTypeID @@HireDate @@EndDate @@BirthDay @@Address 
+@@Tel
+@@Fax
+@@Email 
+@@IsUserID
+@@SipID @@SipPassword</t>
+  </si>
+  <si>
+    <t>Sửa lại câu SQL Insert into. Chỉ dùng cho CustomizeIndex = 51. Thực thi @SQL003 khi thêm mới một người dùng trong Form AS0053</t>
+  </si>
+  <si>
     <t>CustomizeIndex = 51 (Hoàng Trần)
 - Sheet Layout: thêm 2 trường SIP và Mật khẩu
-- Sheet Item Sree: thêm 5 trường Mật khẩu, Nhập lại mật khẩu, SIP, Mật khẩu và Dùng chung
-- Sheet Data Input: Thêm câu @SQL0001 và @SQL0002</t>
-  </si>
-  <si>
-    <t>Textbox này được thêm mới trong màn hình cũ</t>
-  </si>
-  <si>
-    <t>Thêm mới trường SipPassword vào AT1103 áp dụng cho CustomizeIndex 51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thêm mới trường SipID vào AT1103 áp dụng cho CustomizeIndex 51 </t>
+- Sheet Item Sreen: thêm 5 trường Mật khẩu, Nhập lại mật khẩu, SIP, Mật khẩu và Dùng chung
+- Sheet Data Input: Thêm câu @SQL0001, @SQL0002, @SQL0003</t>
   </si>
 </sst>
 </file>
@@ -2275,7 +2311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2619,6 +2655,39 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2628,30 +2697,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2688,15 +2733,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2708,6 +2744,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3135,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:J6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3253,7 +3298,7 @@
       <c r="I5" s="106"/>
       <c r="J5" s="106"/>
     </row>
-    <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="94">
         <v>2</v>
       </c>
@@ -3267,7 +3312,7 @@
         <v>210</v>
       </c>
       <c r="E6" s="110" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="F6" s="111"/>
       <c r="G6" s="111"/>
@@ -3795,15 +3840,23 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
     <mergeCell ref="E26:J26"/>
@@ -3819,23 +3872,15 @@
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
     <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -3852,7 +3897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A47" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
@@ -4692,7 +4737,7 @@
   <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="E25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5679,7 +5724,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:18" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="33" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A27" s="97">
         <v>23</v>
       </c>
@@ -5718,10 +5763,10 @@
       <c r="P27" s="99"/>
       <c r="Q27" s="99"/>
       <c r="R27" s="99" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="33" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A28" s="102">
         <v>24</v>
       </c>
@@ -5760,7 +5805,7 @@
       <c r="P28" s="99"/>
       <c r="Q28" s="99"/>
       <c r="R28" s="99" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="33" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
@@ -7747,8 +7792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47:J47"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A48" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7762,7 +7807,7 @@
     <col min="9" max="9" width="15.28515625" style="23" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" style="23" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" style="23" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="23" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" style="23" customWidth="1"/>
     <col min="13" max="13" width="13" style="23" customWidth="1"/>
     <col min="14" max="15" width="12.7109375" style="23" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="22" customWidth="1"/>
@@ -7896,13 +7941,13 @@
       <c r="G5" s="117" t="s">
         <v>173</v>
       </c>
-      <c r="H5" s="141"/>
-      <c r="I5" s="141"/>
-      <c r="J5" s="142"/>
-      <c r="K5" s="135" t="s">
+      <c r="H5" s="135"/>
+      <c r="I5" s="135"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="146" t="s">
         <v>174</v>
       </c>
-      <c r="L5" s="135" t="s">
+      <c r="L5" s="146" t="s">
         <v>188</v>
       </c>
       <c r="M5" s="37"/>
@@ -7924,12 +7969,12 @@
       </c>
       <c r="E6" s="59"/>
       <c r="F6" s="37"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="144"/>
-      <c r="I6" s="144"/>
-      <c r="J6" s="145"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
+      <c r="G6" s="137"/>
+      <c r="H6" s="138"/>
+      <c r="I6" s="138"/>
+      <c r="J6" s="139"/>
+      <c r="K6" s="147"/>
+      <c r="L6" s="147"/>
       <c r="M6" s="37"/>
       <c r="N6" s="60"/>
       <c r="O6" s="60"/>
@@ -7949,12 +7994,12 @@
       </c>
       <c r="E7" s="59"/>
       <c r="F7" s="37"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="144"/>
-      <c r="I7" s="144"/>
-      <c r="J7" s="145"/>
-      <c r="K7" s="136"/>
-      <c r="L7" s="136"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="147"/>
       <c r="M7" s="37"/>
       <c r="N7" s="60"/>
       <c r="O7" s="60"/>
@@ -7974,12 +8019,12 @@
       </c>
       <c r="E8" s="59"/>
       <c r="F8" s="37"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="144"/>
-      <c r="I8" s="144"/>
-      <c r="J8" s="145"/>
-      <c r="K8" s="136"/>
-      <c r="L8" s="136"/>
+      <c r="G8" s="137"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="147"/>
+      <c r="L8" s="147"/>
       <c r="M8" s="37"/>
       <c r="N8" s="60"/>
       <c r="O8" s="60"/>
@@ -7999,12 +8044,12 @@
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="37"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="144"/>
-      <c r="I9" s="144"/>
-      <c r="J9" s="145"/>
-      <c r="K9" s="136"/>
-      <c r="L9" s="136"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="139"/>
+      <c r="K9" s="147"/>
+      <c r="L9" s="147"/>
       <c r="M9" s="37"/>
       <c r="N9" s="60"/>
       <c r="O9" s="60"/>
@@ -8024,12 +8069,12 @@
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="37"/>
-      <c r="G10" s="143"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="144"/>
-      <c r="J10" s="145"/>
-      <c r="K10" s="136"/>
-      <c r="L10" s="136"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="139"/>
+      <c r="K10" s="147"/>
+      <c r="L10" s="147"/>
       <c r="M10" s="37"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
@@ -8049,12 +8094,12 @@
       </c>
       <c r="E11" s="59"/>
       <c r="F11" s="37"/>
-      <c r="G11" s="143"/>
-      <c r="H11" s="144"/>
-      <c r="I11" s="144"/>
-      <c r="J11" s="145"/>
-      <c r="K11" s="136"/>
-      <c r="L11" s="136"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="138"/>
+      <c r="J11" s="139"/>
+      <c r="K11" s="147"/>
+      <c r="L11" s="147"/>
       <c r="M11" s="37"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
@@ -8074,12 +8119,12 @@
       </c>
       <c r="E12" s="59"/>
       <c r="F12" s="37"/>
-      <c r="G12" s="143"/>
-      <c r="H12" s="144"/>
-      <c r="I12" s="144"/>
-      <c r="J12" s="145"/>
-      <c r="K12" s="136"/>
-      <c r="L12" s="136"/>
+      <c r="G12" s="137"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="138"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="147"/>
+      <c r="L12" s="147"/>
       <c r="M12" s="37"/>
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
@@ -8099,12 +8144,12 @@
       </c>
       <c r="E13" s="59"/>
       <c r="F13" s="37"/>
-      <c r="G13" s="143"/>
-      <c r="H13" s="144"/>
-      <c r="I13" s="144"/>
-      <c r="J13" s="145"/>
-      <c r="K13" s="136"/>
-      <c r="L13" s="136"/>
+      <c r="G13" s="137"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="147"/>
+      <c r="L13" s="147"/>
       <c r="M13" s="37"/>
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
@@ -8124,12 +8169,12 @@
       </c>
       <c r="E14" s="59"/>
       <c r="F14" s="37"/>
-      <c r="G14" s="143"/>
-      <c r="H14" s="144"/>
-      <c r="I14" s="144"/>
-      <c r="J14" s="145"/>
-      <c r="K14" s="136"/>
-      <c r="L14" s="136"/>
+      <c r="G14" s="137"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="139"/>
+      <c r="K14" s="147"/>
+      <c r="L14" s="147"/>
       <c r="M14" s="37"/>
       <c r="N14" s="60"/>
       <c r="O14" s="60"/>
@@ -8149,12 +8194,12 @@
       </c>
       <c r="E15" s="59"/>
       <c r="F15" s="37"/>
-      <c r="G15" s="143"/>
-      <c r="H15" s="144"/>
-      <c r="I15" s="144"/>
-      <c r="J15" s="145"/>
-      <c r="K15" s="136"/>
-      <c r="L15" s="136"/>
+      <c r="G15" s="137"/>
+      <c r="H15" s="138"/>
+      <c r="I15" s="138"/>
+      <c r="J15" s="139"/>
+      <c r="K15" s="147"/>
+      <c r="L15" s="147"/>
       <c r="M15" s="37"/>
       <c r="N15" s="60"/>
       <c r="O15" s="60"/>
@@ -8174,12 +8219,12 @@
       </c>
       <c r="E16" s="59"/>
       <c r="F16" s="37"/>
-      <c r="G16" s="143"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="145"/>
-      <c r="K16" s="136"/>
-      <c r="L16" s="136"/>
+      <c r="G16" s="137"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="139"/>
+      <c r="K16" s="147"/>
+      <c r="L16" s="147"/>
       <c r="M16" s="37"/>
       <c r="N16" s="60"/>
       <c r="O16" s="60"/>
@@ -8199,12 +8244,12 @@
       </c>
       <c r="E17" s="59"/>
       <c r="F17" s="37"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="137"/>
-      <c r="L17" s="137"/>
+      <c r="G17" s="140"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="141"/>
+      <c r="J17" s="142"/>
+      <c r="K17" s="148"/>
+      <c r="L17" s="148"/>
       <c r="M17" s="37"/>
       <c r="N17" s="60"/>
       <c r="O17" s="60"/>
@@ -8224,12 +8269,12 @@
       </c>
       <c r="E18" s="59"/>
       <c r="F18" s="37"/>
-      <c r="G18" s="138" t="s">
+      <c r="G18" s="143" t="s">
         <v>206</v>
       </c>
-      <c r="H18" s="139"/>
-      <c r="I18" s="139"/>
-      <c r="J18" s="140"/>
+      <c r="H18" s="144"/>
+      <c r="I18" s="144"/>
+      <c r="J18" s="145"/>
       <c r="K18" s="86"/>
       <c r="L18" s="86"/>
       <c r="M18" s="80" t="s">
@@ -8253,12 +8298,12 @@
       </c>
       <c r="E19" s="59"/>
       <c r="F19" s="37"/>
-      <c r="G19" s="138" t="s">
+      <c r="G19" s="143" t="s">
         <v>207</v>
       </c>
-      <c r="H19" s="139"/>
-      <c r="I19" s="139"/>
-      <c r="J19" s="140"/>
+      <c r="H19" s="144"/>
+      <c r="I19" s="144"/>
+      <c r="J19" s="145"/>
       <c r="K19" s="86"/>
       <c r="L19" s="86"/>
       <c r="M19" s="80" t="s">
@@ -8282,12 +8327,12 @@
       </c>
       <c r="E20" s="59"/>
       <c r="F20" s="37"/>
-      <c r="G20" s="138" t="s">
+      <c r="G20" s="143" t="s">
         <v>208</v>
       </c>
-      <c r="H20" s="139"/>
-      <c r="I20" s="139"/>
-      <c r="J20" s="140"/>
+      <c r="H20" s="144"/>
+      <c r="I20" s="144"/>
+      <c r="J20" s="145"/>
       <c r="K20" s="87" t="s">
         <v>177</v>
       </c>
@@ -8315,12 +8360,12 @@
       </c>
       <c r="E21" s="59"/>
       <c r="F21" s="37"/>
-      <c r="G21" s="138" t="s">
+      <c r="G21" s="143" t="s">
         <v>209</v>
       </c>
-      <c r="H21" s="139"/>
-      <c r="I21" s="139"/>
-      <c r="J21" s="140"/>
+      <c r="H21" s="144"/>
+      <c r="I21" s="144"/>
+      <c r="J21" s="145"/>
       <c r="K21" s="87" t="s">
         <v>178</v>
       </c>
@@ -8351,9 +8396,9 @@
       <c r="G22" s="117" t="s">
         <v>175</v>
       </c>
-      <c r="H22" s="141"/>
-      <c r="I22" s="141"/>
-      <c r="J22" s="142"/>
+      <c r="H22" s="135"/>
+      <c r="I22" s="135"/>
+      <c r="J22" s="136"/>
       <c r="K22" s="81" t="s">
         <v>174</v>
       </c>
@@ -8379,10 +8424,10 @@
       </c>
       <c r="E23" s="59"/>
       <c r="F23" s="37"/>
-      <c r="G23" s="143"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="144"/>
-      <c r="J23" s="145"/>
+      <c r="G23" s="137"/>
+      <c r="H23" s="138"/>
+      <c r="I23" s="138"/>
+      <c r="J23" s="139"/>
       <c r="K23" s="91" t="s">
         <v>176</v>
       </c>
@@ -8408,10 +8453,10 @@
       </c>
       <c r="E24" s="59"/>
       <c r="F24" s="37"/>
-      <c r="G24" s="143"/>
-      <c r="H24" s="144"/>
-      <c r="I24" s="144"/>
-      <c r="J24" s="145"/>
+      <c r="G24" s="137"/>
+      <c r="H24" s="138"/>
+      <c r="I24" s="138"/>
+      <c r="J24" s="139"/>
       <c r="K24" s="91" t="s">
         <v>177</v>
       </c>
@@ -8437,10 +8482,10 @@
       </c>
       <c r="E25" s="59"/>
       <c r="F25" s="37"/>
-      <c r="G25" s="143"/>
-      <c r="H25" s="144"/>
-      <c r="I25" s="144"/>
-      <c r="J25" s="145"/>
+      <c r="G25" s="137"/>
+      <c r="H25" s="138"/>
+      <c r="I25" s="138"/>
+      <c r="J25" s="139"/>
       <c r="K25" s="91" t="s">
         <v>178</v>
       </c>
@@ -8466,10 +8511,10 @@
       </c>
       <c r="E26" s="59"/>
       <c r="F26" s="37"/>
-      <c r="G26" s="143"/>
-      <c r="H26" s="144"/>
-      <c r="I26" s="144"/>
-      <c r="J26" s="145"/>
+      <c r="G26" s="137"/>
+      <c r="H26" s="138"/>
+      <c r="I26" s="138"/>
+      <c r="J26" s="139"/>
       <c r="K26" s="91" t="s">
         <v>179</v>
       </c>
@@ -8495,10 +8540,10 @@
       </c>
       <c r="E27" s="59"/>
       <c r="F27" s="37"/>
-      <c r="G27" s="143"/>
-      <c r="H27" s="144"/>
-      <c r="I27" s="144"/>
-      <c r="J27" s="145"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="138"/>
+      <c r="I27" s="138"/>
+      <c r="J27" s="139"/>
       <c r="K27" s="91" t="s">
         <v>180</v>
       </c>
@@ -8524,10 +8569,10 @@
       </c>
       <c r="E28" s="59"/>
       <c r="F28" s="37"/>
-      <c r="G28" s="143"/>
-      <c r="H28" s="144"/>
-      <c r="I28" s="144"/>
-      <c r="J28" s="145"/>
+      <c r="G28" s="137"/>
+      <c r="H28" s="138"/>
+      <c r="I28" s="138"/>
+      <c r="J28" s="139"/>
       <c r="K28" s="91" t="s">
         <v>181</v>
       </c>
@@ -8553,10 +8598,10 @@
       </c>
       <c r="E29" s="59"/>
       <c r="F29" s="37"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="144"/>
-      <c r="I29" s="144"/>
-      <c r="J29" s="145"/>
+      <c r="G29" s="137"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="138"/>
+      <c r="J29" s="139"/>
       <c r="K29" s="91" t="s">
         <v>182</v>
       </c>
@@ -8582,10 +8627,10 @@
       </c>
       <c r="E30" s="59"/>
       <c r="F30" s="37"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="144"/>
-      <c r="I30" s="144"/>
-      <c r="J30" s="145"/>
+      <c r="G30" s="137"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="138"/>
+      <c r="J30" s="139"/>
       <c r="K30" s="91" t="s">
         <v>183</v>
       </c>
@@ -8611,10 +8656,10 @@
       </c>
       <c r="E31" s="59"/>
       <c r="F31" s="37"/>
-      <c r="G31" s="143"/>
-      <c r="H31" s="144"/>
-      <c r="I31" s="144"/>
-      <c r="J31" s="145"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="138"/>
+      <c r="I31" s="138"/>
+      <c r="J31" s="139"/>
       <c r="K31" s="91" t="s">
         <v>184</v>
       </c>
@@ -8640,10 +8685,10 @@
       </c>
       <c r="E32" s="59"/>
       <c r="F32" s="37"/>
-      <c r="G32" s="143"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="144"/>
-      <c r="J32" s="145"/>
+      <c r="G32" s="137"/>
+      <c r="H32" s="138"/>
+      <c r="I32" s="138"/>
+      <c r="J32" s="139"/>
       <c r="K32" s="91" t="s">
         <v>185</v>
       </c>
@@ -8669,10 +8714,10 @@
       </c>
       <c r="E33" s="59"/>
       <c r="F33" s="37"/>
-      <c r="G33" s="143"/>
-      <c r="H33" s="144"/>
-      <c r="I33" s="144"/>
-      <c r="J33" s="145"/>
+      <c r="G33" s="137"/>
+      <c r="H33" s="138"/>
+      <c r="I33" s="138"/>
+      <c r="J33" s="139"/>
       <c r="K33" s="91" t="s">
         <v>186</v>
       </c>
@@ -8698,12 +8743,12 @@
       </c>
       <c r="E34" s="59"/>
       <c r="F34" s="37"/>
-      <c r="G34" s="149" t="s">
+      <c r="G34" s="152" t="s">
         <v>199</v>
       </c>
-      <c r="H34" s="150"/>
-      <c r="I34" s="150"/>
-      <c r="J34" s="151"/>
+      <c r="H34" s="153"/>
+      <c r="I34" s="153"/>
+      <c r="J34" s="154"/>
       <c r="K34" s="91" t="s">
         <v>176</v>
       </c>
@@ -8729,10 +8774,10 @@
       </c>
       <c r="E35" s="59"/>
       <c r="F35" s="37"/>
-      <c r="G35" s="152"/>
-      <c r="H35" s="153"/>
-      <c r="I35" s="153"/>
-      <c r="J35" s="154"/>
+      <c r="G35" s="155"/>
+      <c r="H35" s="156"/>
+      <c r="I35" s="156"/>
+      <c r="J35" s="157"/>
       <c r="K35" s="91" t="s">
         <v>177</v>
       </c>
@@ -8758,10 +8803,10 @@
       </c>
       <c r="E36" s="59"/>
       <c r="F36" s="37"/>
-      <c r="G36" s="152"/>
-      <c r="H36" s="153"/>
-      <c r="I36" s="153"/>
-      <c r="J36" s="154"/>
+      <c r="G36" s="155"/>
+      <c r="H36" s="156"/>
+      <c r="I36" s="156"/>
+      <c r="J36" s="157"/>
       <c r="K36" s="91" t="s">
         <v>178</v>
       </c>
@@ -8787,10 +8832,10 @@
       </c>
       <c r="E37" s="59"/>
       <c r="F37" s="37"/>
-      <c r="G37" s="152"/>
-      <c r="H37" s="153"/>
-      <c r="I37" s="153"/>
-      <c r="J37" s="154"/>
+      <c r="G37" s="155"/>
+      <c r="H37" s="156"/>
+      <c r="I37" s="156"/>
+      <c r="J37" s="157"/>
       <c r="K37" s="91" t="s">
         <v>179</v>
       </c>
@@ -8816,10 +8861,10 @@
       </c>
       <c r="E38" s="59"/>
       <c r="F38" s="37"/>
-      <c r="G38" s="152"/>
-      <c r="H38" s="153"/>
-      <c r="I38" s="153"/>
-      <c r="J38" s="154"/>
+      <c r="G38" s="155"/>
+      <c r="H38" s="156"/>
+      <c r="I38" s="156"/>
+      <c r="J38" s="157"/>
       <c r="K38" s="91" t="s">
         <v>180</v>
       </c>
@@ -8845,10 +8890,10 @@
       </c>
       <c r="E39" s="59"/>
       <c r="F39" s="37"/>
-      <c r="G39" s="152"/>
-      <c r="H39" s="153"/>
-      <c r="I39" s="153"/>
-      <c r="J39" s="154"/>
+      <c r="G39" s="155"/>
+      <c r="H39" s="156"/>
+      <c r="I39" s="156"/>
+      <c r="J39" s="157"/>
       <c r="K39" s="91" t="s">
         <v>181</v>
       </c>
@@ -8874,10 +8919,10 @@
       </c>
       <c r="E40" s="59"/>
       <c r="F40" s="37"/>
-      <c r="G40" s="152"/>
-      <c r="H40" s="153"/>
-      <c r="I40" s="153"/>
-      <c r="J40" s="154"/>
+      <c r="G40" s="155"/>
+      <c r="H40" s="156"/>
+      <c r="I40" s="156"/>
+      <c r="J40" s="157"/>
       <c r="K40" s="91" t="s">
         <v>182</v>
       </c>
@@ -8903,10 +8948,10 @@
       </c>
       <c r="E41" s="59"/>
       <c r="F41" s="37"/>
-      <c r="G41" s="152"/>
-      <c r="H41" s="153"/>
-      <c r="I41" s="153"/>
-      <c r="J41" s="154"/>
+      <c r="G41" s="155"/>
+      <c r="H41" s="156"/>
+      <c r="I41" s="156"/>
+      <c r="J41" s="157"/>
       <c r="K41" s="91" t="s">
         <v>183</v>
       </c>
@@ -8932,10 +8977,10 @@
       </c>
       <c r="E42" s="59"/>
       <c r="F42" s="37"/>
-      <c r="G42" s="152"/>
-      <c r="H42" s="153"/>
-      <c r="I42" s="153"/>
-      <c r="J42" s="154"/>
+      <c r="G42" s="155"/>
+      <c r="H42" s="156"/>
+      <c r="I42" s="156"/>
+      <c r="J42" s="157"/>
       <c r="K42" s="91" t="s">
         <v>184</v>
       </c>
@@ -8961,10 +9006,10 @@
       </c>
       <c r="E43" s="59"/>
       <c r="F43" s="37"/>
-      <c r="G43" s="152"/>
-      <c r="H43" s="153"/>
-      <c r="I43" s="153"/>
-      <c r="J43" s="154"/>
+      <c r="G43" s="155"/>
+      <c r="H43" s="156"/>
+      <c r="I43" s="156"/>
+      <c r="J43" s="157"/>
       <c r="K43" s="91" t="s">
         <v>185</v>
       </c>
@@ -8990,10 +9035,10 @@
       </c>
       <c r="E44" s="59"/>
       <c r="F44" s="37"/>
-      <c r="G44" s="152"/>
-      <c r="H44" s="153"/>
-      <c r="I44" s="153"/>
-      <c r="J44" s="154"/>
+      <c r="G44" s="155"/>
+      <c r="H44" s="156"/>
+      <c r="I44" s="156"/>
+      <c r="J44" s="157"/>
       <c r="K44" s="91" t="s">
         <v>186</v>
       </c>
@@ -9019,10 +9064,10 @@
       </c>
       <c r="E45" s="59"/>
       <c r="F45" s="37"/>
-      <c r="G45" s="152"/>
-      <c r="H45" s="153"/>
-      <c r="I45" s="153"/>
-      <c r="J45" s="154"/>
+      <c r="G45" s="155"/>
+      <c r="H45" s="156"/>
+      <c r="I45" s="156"/>
+      <c r="J45" s="157"/>
       <c r="K45" s="91" t="s">
         <v>133</v>
       </c>
@@ -9042,10 +9087,10 @@
       <c r="D46" s="59"/>
       <c r="E46" s="59"/>
       <c r="F46" s="37"/>
-      <c r="G46" s="155"/>
-      <c r="H46" s="156"/>
-      <c r="I46" s="156"/>
-      <c r="J46" s="157"/>
+      <c r="G46" s="158"/>
+      <c r="H46" s="159"/>
+      <c r="I46" s="159"/>
+      <c r="J46" s="160"/>
       <c r="K46" s="81" t="s">
         <v>174</v>
       </c>
@@ -9075,16 +9120,16 @@
       <c r="F47" s="105" t="s">
         <v>237</v>
       </c>
-      <c r="G47" s="146" t="s">
+      <c r="G47" s="149" t="s">
         <v>235</v>
       </c>
-      <c r="H47" s="147"/>
-      <c r="I47" s="147"/>
-      <c r="J47" s="148"/>
+      <c r="H47" s="150"/>
+      <c r="I47" s="150"/>
+      <c r="J47" s="151"/>
       <c r="K47" s="103"/>
       <c r="L47" s="103"/>
       <c r="M47" s="93" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="N47" s="60"/>
       <c r="O47" s="60"/>
@@ -9108,36 +9153,54 @@
       <c r="F48" s="105" t="s">
         <v>238</v>
       </c>
-      <c r="G48" s="146" t="s">
+      <c r="G48" s="149" t="s">
         <v>236</v>
       </c>
-      <c r="H48" s="147"/>
-      <c r="I48" s="147"/>
-      <c r="J48" s="148"/>
+      <c r="H48" s="150"/>
+      <c r="I48" s="150"/>
+      <c r="J48" s="151"/>
       <c r="K48" s="103"/>
       <c r="L48" s="103"/>
       <c r="M48" s="93" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="N48" s="60"/>
       <c r="O48" s="60"/>
     </row>
-    <row r="49" spans="1:15" s="33" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="32">
+    <row r="49" spans="1:15" s="33" customFormat="1" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="102">
         <v>45</v>
       </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="68"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="83"/>
-      <c r="H49" s="84"/>
-      <c r="I49" s="84"/>
-      <c r="J49" s="85"/>
-      <c r="K49" s="81"/>
-      <c r="L49" s="81"/>
-      <c r="M49" s="37"/>
+      <c r="B49" s="102" t="s">
+        <v>219</v>
+      </c>
+      <c r="C49" s="99" t="s">
+        <v>245</v>
+      </c>
+      <c r="D49" s="104" t="s">
+        <v>131</v>
+      </c>
+      <c r="E49" s="104" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="105" t="s">
+        <v>246</v>
+      </c>
+      <c r="G49" s="165" t="s">
+        <v>247</v>
+      </c>
+      <c r="H49" s="166"/>
+      <c r="I49" s="166"/>
+      <c r="J49" s="167"/>
+      <c r="K49" s="103" t="s">
+        <v>248</v>
+      </c>
+      <c r="L49" s="103" t="s">
+        <v>249</v>
+      </c>
+      <c r="M49" s="93" t="s">
+        <v>250</v>
+      </c>
       <c r="N49" s="60"/>
       <c r="O49" s="60"/>
     </row>
@@ -9169,10 +9232,10 @@
       <c r="D51" s="59"/>
       <c r="E51" s="59"/>
       <c r="F51" s="37"/>
-      <c r="G51" s="138"/>
-      <c r="H51" s="139"/>
-      <c r="I51" s="139"/>
-      <c r="J51" s="140"/>
+      <c r="G51" s="143"/>
+      <c r="H51" s="144"/>
+      <c r="I51" s="144"/>
+      <c r="J51" s="145"/>
       <c r="K51" s="56"/>
       <c r="L51" s="56"/>
       <c r="M51" s="37"/>
@@ -9188,10 +9251,10 @@
       <c r="D52" s="59"/>
       <c r="E52" s="59"/>
       <c r="F52" s="37"/>
-      <c r="G52" s="138"/>
-      <c r="H52" s="139"/>
-      <c r="I52" s="139"/>
-      <c r="J52" s="140"/>
+      <c r="G52" s="143"/>
+      <c r="H52" s="144"/>
+      <c r="I52" s="144"/>
+      <c r="J52" s="145"/>
       <c r="K52" s="56"/>
       <c r="L52" s="56"/>
       <c r="M52" s="37"/>
@@ -9207,10 +9270,10 @@
       <c r="D53" s="59"/>
       <c r="E53" s="59"/>
       <c r="F53" s="37"/>
-      <c r="G53" s="138"/>
-      <c r="H53" s="139"/>
-      <c r="I53" s="139"/>
-      <c r="J53" s="140"/>
+      <c r="G53" s="143"/>
+      <c r="H53" s="144"/>
+      <c r="I53" s="144"/>
+      <c r="J53" s="145"/>
       <c r="K53" s="56"/>
       <c r="L53" s="56"/>
       <c r="M53" s="37"/>
@@ -9226,10 +9289,10 @@
       <c r="D54" s="59"/>
       <c r="E54" s="59"/>
       <c r="F54" s="37"/>
-      <c r="G54" s="138"/>
-      <c r="H54" s="139"/>
-      <c r="I54" s="139"/>
-      <c r="J54" s="140"/>
+      <c r="G54" s="143"/>
+      <c r="H54" s="144"/>
+      <c r="I54" s="144"/>
+      <c r="J54" s="145"/>
       <c r="K54" s="56"/>
       <c r="L54" s="56"/>
       <c r="M54" s="37"/>
@@ -9237,12 +9300,15 @@
       <c r="O54" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="G5:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
+  <mergeCells count="20">
+    <mergeCell ref="K5:K17"/>
+    <mergeCell ref="L5:L17"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="G22:J33"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="G34:J46"/>
+    <mergeCell ref="G49:J49"/>
     <mergeCell ref="G54:J54"/>
     <mergeCell ref="G52:J52"/>
     <mergeCell ref="G51:J51"/>
@@ -9250,13 +9316,11 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="G21:J21"/>
-    <mergeCell ref="K5:K17"/>
-    <mergeCell ref="L5:L17"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G22:J33"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="G34:J46"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="G5:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D54">

</xml_diff>